<commit_message>
correction extension dans profil location
correction erreur sur l'extension f40f2a54f06fd30f619bd4ef6d122287ceb3193b
</commit_message>
<xml_diff>
--- a/ig/sd-extension-contact-spécifique-au-site/StructureDefinition-eclaire-location.xlsx
+++ b/ig/sd-extension-contact-spécifique-au-site/StructureDefinition-eclaire-location.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$47</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="303">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-27T17:03:25+00:00</t>
+    <t>2023-07-28T07:09:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -330,7 +330,233 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>Location.extension:eclaire-site-contact-name</t>
+    <t>Location.modifierExtension</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+  </si>
+  <si>
+    <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>Location.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Unique code or number identifying the location to its users</t>
+  </si>
+  <si>
+    <t>Unique code or number identifying the location to its users.</t>
+  </si>
+  <si>
+    <t>Organization label locations in registries, need to keep track of those.</t>
+  </si>
+  <si>
+    <t>.id</t>
+  </si>
+  <si>
+    <t>FiveWs.identifier</t>
+  </si>
+  <si>
+    <t>Location.status</t>
+  </si>
+  <si>
+    <t>active | suspended | inactive</t>
+  </si>
+  <si>
+    <t>The status property covers the general availability of the resource, not the current value which may be covered by the operationStatus, or by a schedule/slots if they are configured for the location.</t>
+  </si>
+  <si>
+    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Indicates whether the location is still in use.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/location-status|4.0.1</t>
+  </si>
+  <si>
+    <t>.statusCode</t>
+  </si>
+  <si>
+    <t>FiveWs.status</t>
+  </si>
+  <si>
+    <t>Location.operationalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>The operational status of the location (typically only for a bed/room)</t>
+  </si>
+  <si>
+    <t>The operational status covers operation values most relevant to beds (but can also apply to rooms/units/chairs/etc. such as an isolation unit/dialysis chair). This typically covers concepts such as contamination, housekeeping, and other activities like maintenance.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.</t>
+  </si>
+  <si>
+    <t>The operational status if the location (where typically a bed/room).</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/ValueSet/v2-0116</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Location.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Name of the location as used by humans</t>
+  </si>
+  <si>
+    <t>Name of the location as used by humans. Does not need to be unique.</t>
+  </si>
+  <si>
+    <t>If the name of a location changes, consider putting the old name in the alias column so that it can still be located through searches.</t>
+  </si>
+  <si>
+    <t>.name</t>
+  </si>
+  <si>
+    <t>Location.alias</t>
+  </si>
+  <si>
+    <t>A list of alternate names that the location is known as, or was known as, in the past</t>
+  </si>
+  <si>
+    <t>A list of alternate names that the location is known as, or was known as, in the past.</t>
+  </si>
+  <si>
+    <t>There are no dates associated with the alias/historic names, as this is not intended to track when names were used, but to assist in searching so that older names can still result in identifying the location.</t>
+  </si>
+  <si>
+    <t>Over time locations and organizations go through many changes and can be known by different names.
+For searching knowing previous names that the location was known by can be very useful.</t>
+  </si>
+  <si>
+    <t>Location.description</t>
+  </si>
+  <si>
+    <t>Additional details about the location that could be displayed as further information to identify the location beyond its name</t>
+  </si>
+  <si>
+    <t>Description of the Location, which helps in finding or referencing the place.</t>
+  </si>
+  <si>
+    <t>Humans need additional information to verify a correct location has been identified.</t>
+  </si>
+  <si>
+    <t>.playingEntity[classCode=PLC determinerCode=INSTANCE].desc</t>
+  </si>
+  <si>
+    <t>Location.mode</t>
+  </si>
+  <si>
+    <t>instance | kind</t>
+  </si>
+  <si>
+    <t>Indicates whether a resource instance represents a specific location or a class of locations.</t>
+  </si>
+  <si>
+    <t>This is labeled as a modifier because whether or not the location is a class of locations changes how it can be used and understood.</t>
+  </si>
+  <si>
+    <t>When using a Location resource for scheduling or orders, we need to be able to refer to a class of Locations instead of a specific Location.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/location-mode|4.0.1</t>
+  </si>
+  <si>
+    <t>.playingEntity[classCode=PLC].determinerCode</t>
+  </si>
+  <si>
+    <t>FiveWs.class</t>
+  </si>
+  <si>
+    <t>Location.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeableConcept
+</t>
+  </si>
+  <si>
+    <t>Type of function performed</t>
+  </si>
+  <si>
+    <t>Indicates the type of function performed at the location.</t>
+  </si>
+  <si>
+    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/ValueSet/v3-ServiceDeliveryLocationRoleType</t>
+  </si>
+  <si>
+    <t>.code</t>
+  </si>
+  <si>
+    <t>Location.telecom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContactPoint
+</t>
+  </si>
+  <si>
+    <t>Contact details of the location</t>
+  </si>
+  <si>
+    <t>The contact details of communication devices available at the location. This can include phone numbers, fax numbers, mobile numbers, email addresses and web sites.</t>
+  </si>
+  <si>
+    <t>.telecom</t>
+  </si>
+  <si>
+    <t>Location.telecom.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>Location.telecom.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Location.telecom.extension:eclaire-site-contact-name</t>
   </si>
   <si>
     <t>eclaire-site-contact-name</t>
@@ -346,213 +572,123 @@
     <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer le nom de contact spécifique au site de recrutement</t>
   </si>
   <si>
-    <t>Location.modifierExtension</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
-  </si>
-  <si>
-    <t>DomainResource.modifierExtension</t>
-  </si>
-  <si>
-    <t>Location.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier
+    <t>Location.telecom.system</t>
+  </si>
+  <si>
+    <t>phone | fax | email | pager | url | sms | other</t>
+  </si>
+  <si>
+    <t>Telecommunications form for contact point - what communications system is required to make use of the contact.</t>
+  </si>
+  <si>
+    <t>Telecommunications form for contact point.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/contact-point-system|4.0.1</t>
+  </si>
+  <si>
+    <t>ContactPoint.system</t>
+  </si>
+  <si>
+    <t>ele-1
+cpt-2</t>
+  </si>
+  <si>
+    <t>./scheme</t>
+  </si>
+  <si>
+    <t>Location.telecom.value</t>
+  </si>
+  <si>
+    <t>The actual contact point details</t>
+  </si>
+  <si>
+    <t>The actual contact point details, in a form that is meaningful to the designated communication system (i.e. phone number or email address).</t>
+  </si>
+  <si>
+    <t>Additional text data such as phone extension numbers, or notes about use of the contact are sometimes included in the value.</t>
+  </si>
+  <si>
+    <t>Need to support legacy numbers that are not in a tightly controlled format.</t>
+  </si>
+  <si>
+    <t>ContactPoint.value</t>
+  </si>
+  <si>
+    <t>./url</t>
+  </si>
+  <si>
+    <t>Location.telecom.use</t>
+  </si>
+  <si>
+    <t>home | work | temp | old | mobile - purpose of this contact point</t>
+  </si>
+  <si>
+    <t>Identifies the purpose for the contact point.</t>
+  </si>
+  <si>
+    <t>Applications can assume that a contact is current unless it explicitly says that it is temporary or old.</t>
+  </si>
+  <si>
+    <t>Need to track the way a person uses this contact, so a user can choose which is appropriate for their purpose.</t>
+  </si>
+  <si>
+    <t>Use of contact point.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/contact-point-use|4.0.1</t>
+  </si>
+  <si>
+    <t>ContactPoint.use</t>
+  </si>
+  <si>
+    <t>unique(./use)</t>
+  </si>
+  <si>
+    <t>Location.telecom.rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positiveInt
 </t>
   </si>
   <si>
-    <t>Unique code or number identifying the location to its users</t>
-  </si>
-  <si>
-    <t>Unique code or number identifying the location to its users.</t>
-  </si>
-  <si>
-    <t>Organization label locations in registries, need to keep track of those.</t>
-  </si>
-  <si>
-    <t>.id</t>
-  </si>
-  <si>
-    <t>FiveWs.identifier</t>
-  </si>
-  <si>
-    <t>Location.status</t>
-  </si>
-  <si>
-    <t>active | suspended | inactive</t>
-  </si>
-  <si>
-    <t>The status property covers the general availability of the resource, not the current value which may be covered by the operationStatus, or by a schedule/slots if they are configured for the location.</t>
-  </si>
-  <si>
-    <t>Note that FHIR strings SHALL NOT exceed 1MB in size</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Indicates whether the location is still in use.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/location-status|4.0.1</t>
-  </si>
-  <si>
-    <t>.statusCode</t>
-  </si>
-  <si>
-    <t>FiveWs.status</t>
-  </si>
-  <si>
-    <t>Location.operationalStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
+    <t>Specify preferred order of use (1 = highest)</t>
+  </si>
+  <si>
+    <t>Specifies a preferred order in which to use a set of contacts. ContactPoints with lower rank values are more preferred than those with higher rank values.</t>
+  </si>
+  <si>
+    <t>Note that rank does not necessarily follow the order in which the contacts are represented in the instance.</t>
+  </si>
+  <si>
+    <t>ContactPoint.rank</t>
+  </si>
+  <si>
+    <t>Location.telecom.period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period
 </t>
   </si>
   <si>
-    <t>The operational status of the location (typically only for a bed/room)</t>
-  </si>
-  <si>
-    <t>The operational status covers operation values most relevant to beds (but can also apply to rooms/units/chairs/etc. such as an isolation unit/dialysis chair). This typically covers concepts such as contamination, housekeeping, and other activities like maintenance.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.</t>
-  </si>
-  <si>
-    <t>The operational status if the location (where typically a bed/room).</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/ValueSet/v2-0116</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>Location.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Name of the location as used by humans</t>
-  </si>
-  <si>
-    <t>Name of the location as used by humans. Does not need to be unique.</t>
-  </si>
-  <si>
-    <t>If the name of a location changes, consider putting the old name in the alias column so that it can still be located through searches.</t>
-  </si>
-  <si>
-    <t>.name</t>
-  </si>
-  <si>
-    <t>Location.alias</t>
-  </si>
-  <si>
-    <t>A list of alternate names that the location is known as, or was known as, in the past</t>
-  </si>
-  <si>
-    <t>A list of alternate names that the location is known as, or was known as, in the past.</t>
-  </si>
-  <si>
-    <t>There are no dates associated with the alias/historic names, as this is not intended to track when names were used, but to assist in searching so that older names can still result in identifying the location.</t>
-  </si>
-  <si>
-    <t>Over time locations and organizations go through many changes and can be known by different names.
-For searching knowing previous names that the location was known by can be very useful.</t>
-  </si>
-  <si>
-    <t>Location.description</t>
-  </si>
-  <si>
-    <t>Additional details about the location that could be displayed as further information to identify the location beyond its name</t>
-  </si>
-  <si>
-    <t>Description of the Location, which helps in finding or referencing the place.</t>
-  </si>
-  <si>
-    <t>Humans need additional information to verify a correct location has been identified.</t>
-  </si>
-  <si>
-    <t>.playingEntity[classCode=PLC determinerCode=INSTANCE].desc</t>
-  </si>
-  <si>
-    <t>Location.mode</t>
-  </si>
-  <si>
-    <t>instance | kind</t>
-  </si>
-  <si>
-    <t>Indicates whether a resource instance represents a specific location or a class of locations.</t>
-  </si>
-  <si>
-    <t>This is labeled as a modifier because whether or not the location is a class of locations changes how it can be used and understood.</t>
-  </si>
-  <si>
-    <t>When using a Location resource for scheduling or orders, we need to be able to refer to a class of Locations instead of a specific Location.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/location-mode|4.0.1</t>
-  </si>
-  <si>
-    <t>.playingEntity[classCode=PLC].determinerCode</t>
-  </si>
-  <si>
-    <t>FiveWs.class</t>
-  </si>
-  <si>
-    <t>Location.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CodeableConcept
-</t>
-  </si>
-  <si>
-    <t>Type of function performed</t>
-  </si>
-  <si>
-    <t>Indicates the type of function performed at the location.</t>
-  </si>
-  <si>
-    <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/ValueSet/v3-ServiceDeliveryLocationRoleType</t>
-  </si>
-  <si>
-    <t>.code</t>
-  </si>
-  <si>
-    <t>Location.telecom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ContactPoint
-</t>
-  </si>
-  <si>
-    <t>Contact details of the location</t>
-  </si>
-  <si>
-    <t>The contact details of communication devices available at the location. This can include phone numbers, fax numbers, mobile numbers, email addresses and web sites.</t>
+    <t>Time period when the contact point was/is in use</t>
+  </si>
+  <si>
+    <t>Time period when the contact point was/is in use.</t>
+  </si>
+  <si>
+    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
+Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
+  </si>
+  <si>
+    <t>ContactPoint.period</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}</t>
-  </si>
-  <si>
-    <t>.telecom</t>
+per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
+  </si>
+  <si>
+    <t>./usablePeriod[type="IVL&lt;TS&gt;"]</t>
   </si>
   <si>
     <t>Location.address</t>
@@ -623,22 +759,7 @@
     <t>Location.position.id</t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
     <t>Location.position.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Location.position.modifierExtension</t>
@@ -1153,7 +1274,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL40"/>
+  <dimension ref="A1:AL47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1162,7 +1283,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.98046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.5" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="42.98046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="24.55859375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -2065,41 +2186,43 @@
         <v>99</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="I9" t="s" s="2">
-        <v>34</v>
-      </c>
       <c r="J9" t="s" s="2">
         <v>34</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="N9" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="O9" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="M9" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
         <v>34</v>
       </c>
@@ -2135,19 +2258,19 @@
         <v>34</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>35</v>
@@ -2162,7 +2285,7 @@
         <v>98</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>34</v>
@@ -2177,7 +2300,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2190,25 +2313,23 @@
         <v>34</v>
       </c>
       <c r="I10" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="J10" t="s" s="2">
-        <v>34</v>
-      </c>
       <c r="K10" t="s" s="2">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>93</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>34</v>
@@ -2245,19 +2366,19 @@
         <v>34</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="AD10" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>35</v>
@@ -2269,21 +2390,21 @@
         <v>54</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>34</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2294,30 +2415,30 @@
         <v>35</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s" s="2">
         <v>43</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" t="s" s="2">
         <v>113</v>
       </c>
+      <c r="N11" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
         <v>34</v>
       </c>
@@ -2341,13 +2462,13 @@
         <v>34</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="AA11" t="s" s="2">
         <v>34</v>
@@ -2365,13 +2486,13 @@
         <v>34</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>54</v>
@@ -2380,18 +2501,18 @@
         <v>55</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2408,22 +2529,22 @@
         <v>34</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J12" t="s" s="2">
         <v>43</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" t="s" s="2">
@@ -2449,31 +2570,31 @@
         <v>34</v>
       </c>
       <c r="X12" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF12" t="s" s="2">
         <v>120</v>
-      </c>
-      <c r="Y12" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>116</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>35</v>
@@ -2488,18 +2609,18 @@
         <v>55</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2522,16 +2643,16 @@
         <v>43</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -2557,13 +2678,13 @@
         <v>34</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>131</v>
+        <v>34</v>
       </c>
       <c r="AA13" t="s" s="2">
         <v>34</v>
@@ -2581,7 +2702,7 @@
         <v>34</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>35</v>
@@ -2596,18 +2717,18 @@
         <v>55</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>124</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2618,7 +2739,7 @@
         <v>35</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>34</v>
@@ -2627,10 +2748,10 @@
         <v>34</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L14" t="s" s="2">
         <v>135</v>
@@ -2641,7 +2762,9 @@
       <c r="N14" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" t="s" s="2">
+        <v>138</v>
+      </c>
       <c r="P14" t="s" s="2">
         <v>34</v>
       </c>
@@ -2689,13 +2812,13 @@
         <v>34</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>54</v>
@@ -2704,7 +2827,7 @@
         <v>55</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>34</v>
@@ -2726,7 +2849,7 @@
         <v>35</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>34</v>
@@ -2735,10 +2858,10 @@
         <v>34</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L15" t="s" s="2">
         <v>140</v>
@@ -2747,10 +2870,10 @@
         <v>141</v>
       </c>
       <c r="N15" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O15" t="s" s="2">
         <v>142</v>
-      </c>
-      <c r="O15" t="s" s="2">
-        <v>143</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>34</v>
@@ -2805,7 +2928,7 @@
         <v>35</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>54</v>
@@ -2814,7 +2937,7 @@
         <v>55</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>34</v>
@@ -2848,7 +2971,7 @@
         <v>43</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>134</v>
+        <v>65</v>
       </c>
       <c r="L16" t="s" s="2">
         <v>145</v>
@@ -2857,10 +2980,10 @@
         <v>146</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>34</v>
@@ -2885,13 +3008,13 @@
         <v>34</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>34</v>
@@ -2924,18 +3047,18 @@
         <v>55</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>34</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -2946,7 +3069,7 @@
         <v>35</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>34</v>
@@ -2958,20 +3081,18 @@
         <v>43</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>153</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
         <v>34</v>
       </c>
@@ -2995,13 +3116,13 @@
         <v>34</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>34</v>
@@ -3019,13 +3140,13 @@
         <v>34</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>54</v>
@@ -3034,18 +3155,18 @@
         <v>55</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3065,20 +3186,18 @@
         <v>34</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>161</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
         <v>34</v>
@@ -3103,31 +3222,31 @@
         <v>34</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="Y18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE18" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF18" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="Z18" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="AA18" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AB18" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AC18" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AD18" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AE18" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AF18" t="s" s="2">
-        <v>157</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>35</v>
@@ -3139,13 +3258,13 @@
         <v>54</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>164</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>156</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" hidden="true">
@@ -3164,7 +3283,7 @@
         <v>35</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>34</v>
@@ -3176,13 +3295,13 @@
         <v>34</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>168</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3233,22 +3352,22 @@
         <v>34</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>34</v>
@@ -3256,21 +3375,21 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>34</v>
@@ -3282,20 +3401,18 @@
         <v>34</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>176</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>34</v>
       </c>
@@ -3331,16 +3448,16 @@
         <v>34</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="AC20" t="s" s="2">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="AD20" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>171</v>
@@ -3349,16 +3466,16 @@
         <v>35</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>177</v>
+        <v>56</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>34</v>
@@ -3366,12 +3483,14 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="D21" t="s" s="2">
         <v>34</v>
       </c>
@@ -3383,29 +3502,25 @@
         <v>42</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>34</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="O21" t="s" s="2">
-        <v>181</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
         <v>34</v>
       </c>
@@ -3429,13 +3544,13 @@
         <v>34</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>182</v>
+        <v>34</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>183</v>
+        <v>34</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>184</v>
+        <v>34</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>34</v>
@@ -3453,33 +3568,33 @@
         <v>34</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>185</v>
+        <v>34</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>156</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3499,21 +3614,21 @@
         <v>34</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>187</v>
+        <v>65</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="N22" s="2"/>
-      <c r="O22" t="s" s="2">
-        <v>190</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
         <v>34</v>
       </c>
@@ -3537,13 +3652,13 @@
         <v>34</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>34</v>
+        <v>180</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>34</v>
+        <v>181</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>34</v>
@@ -3561,7 +3676,7 @@
         <v>34</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>35</v>
@@ -3570,13 +3685,13 @@
         <v>42</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>34</v>
@@ -3584,10 +3699,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3607,19 +3722,23 @@
         <v>34</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="O23" t="s" s="2">
+        <v>189</v>
+      </c>
       <c r="P23" t="s" s="2">
         <v>34</v>
       </c>
@@ -3667,7 +3786,7 @@
         <v>34</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>35</v>
@@ -3676,13 +3795,13 @@
         <v>42</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>34</v>
@@ -3690,44 +3809,46 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="O24" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="O24" t="s" s="2">
+        <v>196</v>
+      </c>
       <c r="P24" t="s" s="2">
         <v>34</v>
       </c>
@@ -3751,46 +3872,46 @@
         <v>34</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="Z24" t="s" s="2">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="AA24" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="AD24" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>34</v>
@@ -3798,46 +3919,44 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="O25" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
         <v>34</v>
       </c>
@@ -3885,22 +4004,22 @@
         <v>34</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>34</v>
@@ -3908,10 +4027,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -3919,7 +4038,7 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>42</v>
@@ -3931,19 +4050,19 @@
         <v>34</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -3993,10 +4112,10 @@
         <v>34</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>42</v>
@@ -4005,10 +4124,10 @@
         <v>54</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>34</v>
@@ -4016,10 +4135,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4027,7 +4146,7 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>42</v>
@@ -4042,18 +4161,20 @@
         <v>34</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="O27" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="O27" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P27" t="s" s="2">
         <v>34</v>
       </c>
@@ -4101,10 +4222,10 @@
         <v>34</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>42</v>
@@ -4116,7 +4237,7 @@
         <v>55</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>34</v>
@@ -4124,10 +4245,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4147,21 +4268,23 @@
         <v>34</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="O28" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="O28" t="s" s="2">
+        <v>225</v>
+      </c>
       <c r="P28" t="s" s="2">
         <v>34</v>
       </c>
@@ -4185,13 +4308,13 @@
         <v>34</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>34</v>
+        <v>227</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>34</v>
@@ -4209,7 +4332,7 @@
         <v>34</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>35</v>
@@ -4224,18 +4347,18 @@
         <v>55</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>34</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4255,22 +4378,20 @@
         <v>34</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>220</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>34</v>
@@ -4319,7 +4440,7 @@
         <v>34</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>35</v>
@@ -4331,10 +4452,10 @@
         <v>54</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>222</v>
+        <v>55</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>34</v>
@@ -4342,10 +4463,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4368,20 +4489,16 @@
         <v>34</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>225</v>
+        <v>129</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>226</v>
+        <v>166</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O30" t="s" s="2">
-        <v>229</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>34</v>
       </c>
@@ -4429,7 +4546,7 @@
         <v>34</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>224</v>
+        <v>168</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>35</v>
@@ -4438,13 +4555,13 @@
         <v>42</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>222</v>
+        <v>34</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>230</v>
+        <v>63</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>34</v>
@@ -4452,14 +4569,14 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -4478,16 +4595,16 @@
         <v>34</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>187</v>
+        <v>90</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>232</v>
+        <v>91</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>233</v>
+        <v>170</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>234</v>
+        <v>93</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -4525,19 +4642,19 @@
         <v>34</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="AD31" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>35</v>
@@ -4549,10 +4666,10 @@
         <v>54</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>235</v>
+        <v>56</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>34</v>
@@ -4560,42 +4677,46 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>34</v>
+        <v>239</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="O32" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="P32" t="s" s="2">
         <v>34</v>
       </c>
@@ -4643,22 +4764,22 @@
         <v>34</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>195</v>
+        <v>242</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>34</v>
@@ -4666,21 +4787,21 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>34</v>
@@ -4692,16 +4813,16 @@
         <v>34</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>90</v>
+        <v>244</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>91</v>
+        <v>245</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>93</v>
+        <v>247</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -4739,34 +4860,34 @@
         <v>34</v>
       </c>
       <c r="AB33" t="s" s="2">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="AC33" t="s" s="2">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="AD33" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>56</v>
+        <v>248</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>34</v>
@@ -4774,46 +4895,44 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>90</v>
+        <v>244</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>201</v>
+        <v>250</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>202</v>
+        <v>251</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="O34" t="s" s="2">
-        <v>107</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>34</v>
       </c>
@@ -4861,22 +4980,22 @@
         <v>34</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>54</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>56</v>
+        <v>248</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>34</v>
@@ -4884,10 +5003,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -4898,7 +5017,7 @@
         <v>35</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>34</v>
@@ -4910,16 +5029,16 @@
         <v>34</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>65</v>
+        <v>244</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>119</v>
+        <v>247</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -4945,13 +5064,13 @@
         <v>34</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>242</v>
+        <v>34</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>243</v>
+        <v>34</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>34</v>
@@ -4969,13 +5088,13 @@
         <v>34</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>54</v>
@@ -4984,7 +5103,7 @@
         <v>55</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>34</v>
@@ -4992,10 +5111,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5015,19 +5134,23 @@
         <v>34</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>34</v>
       </c>
@@ -5075,7 +5198,7 @@
         <v>34</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>35</v>
@@ -5087,10 +5210,10 @@
         <v>54</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>55</v>
+        <v>261</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>34</v>
@@ -5098,10 +5221,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5124,16 +5247,20 @@
         <v>34</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O37" t="s" s="2">
+        <v>268</v>
+      </c>
       <c r="P37" t="s" s="2">
         <v>34</v>
       </c>
@@ -5181,7 +5308,7 @@
         <v>34</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>35</v>
@@ -5193,10 +5320,10 @@
         <v>54</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>55</v>
+        <v>261</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>34</v>
@@ -5204,10 +5331,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5218,7 +5345,7 @@
         <v>35</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>34</v>
@@ -5230,15 +5357,17 @@
         <v>34</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>34</v>
@@ -5287,13 +5416,13 @@
         <v>34</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>54</v>
@@ -5302,7 +5431,7 @@
         <v>55</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>34</v>
@@ -5310,10 +5439,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5336,17 +5465,15 @@
         <v>34</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>256</v>
+        <v>166</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>119</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
         <v>34</v>
@@ -5395,7 +5522,7 @@
         <v>34</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>255</v>
+        <v>168</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>35</v>
@@ -5404,10 +5531,10 @@
         <v>42</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>63</v>
@@ -5418,14 +5545,14 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -5444,20 +5571,18 @@
         <v>34</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>259</v>
+        <v>90</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>260</v>
+        <v>91</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>261</v>
+        <v>170</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O40" t="s" s="2">
-        <v>262</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>34</v>
       </c>
@@ -5493,19 +5618,19 @@
         <v>34</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="AC40" t="s" s="2">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="AD40" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>258</v>
+        <v>171</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>35</v>
@@ -5517,17 +5642,771 @@
         <v>54</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>222</v>
+        <v>98</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>263</v>
+        <v>56</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>34</v>
       </c>
     </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G41" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="O41" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="P41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q41" s="2"/>
+      <c r="R41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q43" s="2"/>
+      <c r="R43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" hidden="true">
+      <c r="A44" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q44" s="2"/>
+      <c r="R44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" hidden="true">
+      <c r="A45" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q45" s="2"/>
+      <c r="R45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" hidden="true">
+      <c r="A46" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q46" s="2"/>
+      <c r="R46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" hidden="true">
+      <c r="A47" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O47" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="P47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q47" s="2"/>
+      <c r="R47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AL40">
+  <autoFilter ref="A1:AL47">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5537,7 +6416,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI39">
+  <conditionalFormatting sqref="A2:AI46">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>